<commit_message>
AutoCommit_11 апреля 2024 г. 22:21:44_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1222_ОпСис_\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ОИБАС1222\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="42">
   <si>
-    <t>2ОИБАС1222: Операционные системы (Сибирев И. В.) - I семестр</t>
-  </si>
-  <si>
     <t>Алигишиев Ибрагим</t>
   </si>
   <si>
@@ -144,7 +141,10 @@
     <t>Инд8</t>
   </si>
   <si>
-    <t>Сумма</t>
+    <t>Инд9</t>
+  </si>
+  <si>
+    <t>Инд10</t>
   </si>
 </sst>
 </file>
@@ -228,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -259,6 +259,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -563,13 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="R34" sqref="R34"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -577,74 +580,102 @@
     <col min="1" max="1" width="5.1796875" customWidth="1"/>
     <col min="2" max="2" width="24.453125" customWidth="1"/>
     <col min="3" max="3" width="29.1796875" customWidth="1"/>
-    <col min="4" max="9" width="5.1796875" customWidth="1"/>
+    <col min="4" max="12" width="5.36328125" customWidth="1"/>
+    <col min="14" max="17" width="5.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="9" t="s">
+    <row r="1" spans="1:17" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="3"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="3"/>
       <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <f>IF(B3=C3,A2+1,"-------------------")</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="H3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="4">
+        <v>5</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="5">
+        <v>5</v>
+      </c>
+      <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="Q3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="4">
+        <v>5</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <f>IF(B4=C4,A3+1,"-------------------")</f>
-        <v>1</v>
+        <f t="shared" ref="A4:A30" si="0">IF(B4=C4,A3+1,"-------------------")</f>
+        <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>1</v>
@@ -656,32 +687,24 @@
       <c r="E4" s="4">
         <v>5</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="5">
+      <c r="F4" s="4">
         <v>5</v>
       </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="L4" s="4">
-        <v>5</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q4">
-        <f>SUM(D4:O4)</f>
-        <v>20</v>
-      </c>
-      <c r="R4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="4">
+        <v>5</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A31" si="0">IF(B5=C5,A4+1,"-------------------")</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>2</v>
@@ -699,25 +722,18 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="L5" s="4">
-        <v>5</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="9">
-        <f t="shared" ref="Q5:Q40" si="1">SUM(D5:O5)</f>
-        <v>20</v>
-      </c>
-      <c r="R5">
+      <c r="N5" s="4">
+        <v>5</v>
+      </c>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <f t="shared" si="0"/>
-        <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>3</v>
@@ -729,31 +745,22 @@
       <c r="E6" s="4">
         <v>5</v>
       </c>
-      <c r="F6" s="4">
-        <v>5</v>
-      </c>
+      <c r="F6" s="2"/>
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="L6" s="4">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="4">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="9">
-        <f t="shared" si="1"/>
-        <v>18</v>
-      </c>
-      <c r="R6">
+      <c r="N6" s="4">
+        <v>5</v>
+      </c>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>4</v>
@@ -766,28 +773,22 @@
         <v>5</v>
       </c>
       <c r="F7" s="2"/>
+      <c r="G7" s="5">
+        <v>5</v>
+      </c>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-      <c r="L7" s="4">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="4">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="9">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="R7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N7" s="4">
+        <v>5</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>5</v>
@@ -795,34 +796,31 @@
       <c r="C8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
       <c r="E8" s="4">
         <v>5</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="5">
-        <v>5</v>
-      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="L8" s="4">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="Q8" s="9">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="R8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N8" s="4">
+        <v>5</v>
+      </c>
+      <c r="O8" s="5">
+        <v>5</v>
+      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>6</v>
@@ -836,32 +834,33 @@
       <c r="E9" s="4">
         <v>5</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="4">
-        <v>5</v>
-      </c>
-      <c r="M9" s="5">
-        <v>5</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="R9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="4">
+        <v>5</v>
+      </c>
+      <c r="J9" s="4">
+        <v>5</v>
+      </c>
+      <c r="K9" s="4">
+        <v>5</v>
+      </c>
+      <c r="M9" s="14">
+        <v>5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>5</v>
+      </c>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>7</v>
@@ -878,34 +877,19 @@
       <c r="F10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="4">
-        <v>5</v>
-      </c>
-      <c r="J10" s="4">
-        <v>5</v>
-      </c>
-      <c r="K10" s="4">
-        <v>5</v>
-      </c>
-      <c r="L10" s="4">
-        <v>5</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q10" s="9">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="R10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="N10" s="4">
+        <v>5</v>
+      </c>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>8</v>
@@ -916,32 +900,26 @@
       <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="4">
-        <v>5</v>
-      </c>
-      <c r="F11" s="4">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="5">
         <v>5</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="4">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="Q11" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R11">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="4">
+        <v>5</v>
+      </c>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>9</v>
@@ -949,36 +927,28 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="4">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="5">
-        <v>5</v>
-      </c>
-      <c r="I12" s="8"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4">
+        <v>5</v>
+      </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="4">
-        <v>5</v>
-      </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q12" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>10</v>
@@ -986,35 +956,34 @@
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
       <c r="E13" s="4">
         <v>5</v>
       </c>
       <c r="F13" s="4">
         <v>5</v>
       </c>
-      <c r="I13" s="4">
-        <v>5</v>
-      </c>
+      <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="2"/>
+      <c r="M13">
+        <v>5</v>
+      </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="5">
+        <v>5</v>
+      </c>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>11</v>
@@ -1034,26 +1003,16 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="5">
-        <v>5</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q14" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="R14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N14" s="4">
+        <v>5</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>12</v>
@@ -1061,35 +1020,32 @@
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="4">
-        <v>5</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="4">
         <v>5</v>
       </c>
-      <c r="F15" s="4">
-        <v>5</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="4">
-        <v>5</v>
-      </c>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="Q15" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R15">
+      <c r="F15" s="2"/>
+      <c r="I15" s="8">
+        <v>5</v>
+      </c>
+      <c r="J15" s="8">
+        <v>5</v>
+      </c>
+      <c r="K15" s="8">
+        <v>5</v>
+      </c>
+      <c r="N15" s="4">
+        <v>5</v>
+      </c>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>13</v>
@@ -1098,81 +1054,52 @@
         <v>13</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="4">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="I16" s="8">
-        <v>5</v>
-      </c>
-      <c r="J16" s="8">
-        <v>5</v>
-      </c>
-      <c r="K16" s="8">
-        <v>5</v>
-      </c>
-      <c r="L16" s="4">
-        <v>5</v>
-      </c>
-      <c r="N16" s="2"/>
-      <c r="O16" s="4">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="9">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="R16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="4">
+        <v>5</v>
+      </c>
+      <c r="G16" s="4">
+        <v>5</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="N16" s="4">
+        <v>5</v>
+      </c>
+      <c r="O16" s="5">
+        <v>5</v>
+      </c>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="C17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="4">
-        <v>5</v>
-      </c>
-      <c r="G17" s="4">
-        <v>5</v>
-      </c>
-      <c r="H17" s="4">
-        <v>5</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="4">
-        <v>5</v>
-      </c>
-      <c r="M17" s="5">
-        <v>5</v>
-      </c>
-      <c r="N17" s="2"/>
-      <c r="O17" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q17" s="9">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="R17">
-        <v>5</v>
-      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
     </row>
     <row r="18" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>15</v>
@@ -1183,46 +1110,57 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="L18" s="12"/>
       <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="Q18" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R18" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="10">
-        <f t="shared" si="0"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+    </row>
+    <row r="19" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="C19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="Q19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R19" s="11">
-        <v>0</v>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4">
+        <v>5</v>
+      </c>
+      <c r="I19" s="4">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4">
+        <v>5</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5</v>
+      </c>
+      <c r="N19" s="4">
+        <v>5</v>
+      </c>
+      <c r="O19" s="7">
+        <v>5</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>17</v>
@@ -1239,40 +1177,19 @@
       <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="H20" s="4">
-        <v>5</v>
-      </c>
-      <c r="I20" s="4">
-        <v>5</v>
-      </c>
-      <c r="J20" s="4">
-        <v>5</v>
-      </c>
-      <c r="K20" s="4">
-        <v>5</v>
-      </c>
-      <c r="L20" s="4">
-        <v>5</v>
-      </c>
-      <c r="M20" s="7">
-        <v>5</v>
-      </c>
-      <c r="N20" s="2"/>
-      <c r="O20" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q20" s="9">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="R20">
-        <v>5</v>
-      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="N20" s="4">
+        <v>5</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>18</v>
@@ -1289,26 +1206,23 @@
       <c r="F21" s="4">
         <v>5</v>
       </c>
-      <c r="I21" s="8"/>
+      <c r="I21" s="4">
+        <v>5</v>
+      </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-      <c r="L21" s="4">
-        <v>5</v>
-      </c>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="Q21" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R21">
-        <v>4</v>
+      <c r="N21" s="4">
+        <v>5</v>
+      </c>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>19</v>
@@ -1316,39 +1230,31 @@
       <c r="C22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="4">
-        <v>5</v>
-      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="4">
         <v>5</v>
       </c>
       <c r="F22" s="4">
         <v>5</v>
       </c>
-      <c r="I22" s="4">
-        <v>5</v>
-      </c>
+      <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="L22" s="4">
-        <v>5</v>
-      </c>
-      <c r="N22" s="2"/>
-      <c r="O22" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="9">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="R22">
+      <c r="N22" s="4">
+        <v>5</v>
+      </c>
+      <c r="O22" s="5">
+        <v>5</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>20</v>
@@ -1356,38 +1262,36 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
       <c r="E23" s="4">
         <v>5</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F23" s="2"/>
+      <c r="G23" s="5">
         <v>5</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="L23" s="4">
-        <v>5</v>
-      </c>
-      <c r="M23" s="5">
-        <v>5</v>
-      </c>
-      <c r="N23" s="2"/>
-      <c r="O23" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q23" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="R23">
+      <c r="N23" s="4">
+        <v>5</v>
+      </c>
+      <c r="O23" s="5">
+        <v>5</v>
+      </c>
+      <c r="P23" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>21</v>
@@ -1395,23 +1299,26 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="4">
-        <v>5</v>
-      </c>
+      <c r="D24" s="2"/>
       <c r="E24" s="4">
         <v>5</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="G24" s="5">
-        <v>5</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="4">
-        <v>5</v>
-      </c>
-      <c r="M24" s="5">
+      <c r="F24" s="4">
+        <v>5</v>
+      </c>
+      <c r="G24" s="4">
+        <v>5</v>
+      </c>
+      <c r="H24" s="4">
+        <v>5</v>
+      </c>
+      <c r="I24" s="4">
+        <v>5</v>
+      </c>
+      <c r="J24" s="4">
+        <v>5</v>
+      </c>
+      <c r="K24" s="4">
         <v>5</v>
       </c>
       <c r="N24" s="4">
@@ -1420,18 +1327,18 @@
       <c r="O24" s="4">
         <v>5</v>
       </c>
-      <c r="Q24" s="9">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="R24">
-        <v>5</v>
-      </c>
+      <c r="P24" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>5</v>
+      </c>
+      <c r="R24" s="13"/>
     </row>
     <row r="25" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>22</v>
@@ -1439,52 +1346,31 @@
       <c r="C25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="4">
+        <v>5</v>
+      </c>
       <c r="E25" s="4">
         <v>5</v>
       </c>
       <c r="F25" s="4">
         <v>5</v>
       </c>
-      <c r="G25" s="4">
-        <v>5</v>
-      </c>
-      <c r="H25" s="4">
-        <v>5</v>
-      </c>
-      <c r="I25" s="4">
-        <v>5</v>
-      </c>
-      <c r="J25" s="4">
-        <v>5</v>
-      </c>
-      <c r="K25" s="4">
-        <v>5</v>
-      </c>
-      <c r="L25" s="4">
-        <v>5</v>
-      </c>
-      <c r="M25" s="4">
-        <v>5</v>
-      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
       <c r="N25" s="4">
         <v>5</v>
       </c>
-      <c r="O25" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q25" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R25" s="13">
-        <v>5</v>
-      </c>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="4">
+        <v>5</v>
+      </c>
+      <c r="R25" s="13"/>
     </row>
     <row r="26" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>23</v>
@@ -1504,25 +1390,22 @@
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-      <c r="L26" s="4">
-        <v>5</v>
-      </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="9">
-        <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="R26" s="13">
-        <v>5</v>
-      </c>
+      <c r="N26" s="4">
+        <v>5</v>
+      </c>
+      <c r="O26" s="5">
+        <v>5</v>
+      </c>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="4">
+        <v>5</v>
+      </c>
+      <c r="R26" s="13"/>
     </row>
     <row r="27" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>24</v>
@@ -1539,31 +1422,36 @@
       <c r="F27" s="4">
         <v>5</v>
       </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="4">
-        <v>5</v>
-      </c>
-      <c r="M27" s="5">
-        <v>5</v>
-      </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q27" s="9">
-        <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="R27" s="13">
+      <c r="G27" s="5">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5">
+        <v>5</v>
+      </c>
+      <c r="I27" s="4">
+        <v>5</v>
+      </c>
+      <c r="J27" s="4">
+        <v>5</v>
+      </c>
+      <c r="K27" s="4">
+        <v>5</v>
+      </c>
+      <c r="N27" s="4">
+        <v>5</v>
+      </c>
+      <c r="O27" s="5">
+        <v>5</v>
+      </c>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>25</v>
@@ -1571,52 +1459,29 @@
       <c r="C28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="4">
-        <v>5</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="4">
         <v>5</v>
       </c>
       <c r="F28" s="4">
         <v>5</v>
       </c>
-      <c r="G28" s="5">
-        <v>5</v>
-      </c>
-      <c r="H28" s="5">
-        <v>5</v>
-      </c>
-      <c r="I28" s="4">
-        <v>5</v>
-      </c>
-      <c r="J28" s="4">
-        <v>5</v>
-      </c>
-      <c r="K28" s="4">
-        <v>5</v>
-      </c>
-      <c r="L28" s="4">
-        <v>5</v>
-      </c>
-      <c r="M28" s="5">
-        <v>5</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="O28" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q28" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R28">
-        <v>5</v>
-      </c>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="N28" s="4">
+        <v>5</v>
+      </c>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="4">
+        <v>5</v>
+      </c>
+      <c r="R28" s="13"/>
     </row>
     <row r="29" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>26</v>
@@ -1625,34 +1490,29 @@
         <v>26</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="4">
-        <v>5</v>
-      </c>
-      <c r="F29" s="4">
-        <v>5</v>
-      </c>
-      <c r="I29" s="8"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="I29" s="8">
+        <v>5</v>
+      </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="4">
-        <v>5</v>
-      </c>
-      <c r="N29" s="2"/>
-      <c r="O29" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q29" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R29" s="13">
-        <v>4</v>
-      </c>
+      <c r="N29" s="4">
+        <v>5</v>
+      </c>
+      <c r="P29" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="13"/>
     </row>
     <row r="30" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>27</v>
@@ -1660,42 +1520,44 @@
       <c r="C30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30">
-        <v>5</v>
-      </c>
-      <c r="I30" s="8">
-        <v>5</v>
-      </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="4">
+      <c r="D30" s="4">
+        <v>5</v>
+      </c>
+      <c r="E30" s="4">
+        <v>5</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5</v>
+      </c>
+      <c r="G30" s="6">
+        <v>5</v>
+      </c>
+      <c r="H30" s="6">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4">
+        <v>5</v>
+      </c>
+      <c r="J30" s="4">
+        <v>5</v>
+      </c>
+      <c r="K30" s="4">
         <v>5</v>
       </c>
       <c r="N30" s="4">
         <v>5</v>
       </c>
-      <c r="O30" s="2"/>
-      <c r="Q30" s="9">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="R30" s="13">
-        <v>3</v>
+      <c r="O30" s="6">
+        <v>5</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="4">
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="4">
         <v>5</v>
@@ -1721,27 +1583,20 @@
       <c r="K31" s="4">
         <v>5</v>
       </c>
-      <c r="L31" s="4">
-        <v>5</v>
-      </c>
-      <c r="M31" s="6">
-        <v>5</v>
-      </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q31" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R31">
+      <c r="N31" s="4">
+        <v>5</v>
+      </c>
+      <c r="O31" s="6">
+        <v>5</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="4">
         <v>5</v>
@@ -1767,27 +1622,20 @@
       <c r="K32" s="4">
         <v>5</v>
       </c>
-      <c r="L32" s="4">
-        <v>5</v>
-      </c>
-      <c r="M32" s="6">
-        <v>5</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q32" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N32" s="4">
+        <v>5</v>
+      </c>
+      <c r="O32" s="6">
+        <v>5</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="4">
         <v>5</v>
@@ -1813,27 +1661,20 @@
       <c r="K33" s="4">
         <v>5</v>
       </c>
-      <c r="L33" s="4">
-        <v>5</v>
-      </c>
-      <c r="M33" s="6">
-        <v>5</v>
-      </c>
-      <c r="N33" s="2"/>
-      <c r="O33" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q33" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N33" s="4">
+        <v>5</v>
+      </c>
+      <c r="O33" s="6">
+        <v>5</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="4">
         <v>5</v>
@@ -1859,27 +1700,20 @@
       <c r="K34" s="4">
         <v>5</v>
       </c>
-      <c r="L34" s="4">
-        <v>5</v>
-      </c>
-      <c r="M34" s="6">
-        <v>5</v>
-      </c>
-      <c r="N34" s="2"/>
-      <c r="O34" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q34" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R34">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N34" s="4">
+        <v>5</v>
+      </c>
+      <c r="O34" s="6">
+        <v>5</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="4">
         <v>5</v>
@@ -1905,27 +1739,20 @@
       <c r="K35" s="4">
         <v>5</v>
       </c>
-      <c r="L35" s="4">
-        <v>5</v>
-      </c>
-      <c r="M35" s="6">
-        <v>5</v>
-      </c>
-      <c r="N35" s="2"/>
-      <c r="O35" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q35" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R35">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N35" s="4">
+        <v>5</v>
+      </c>
+      <c r="O35" s="6">
+        <v>5</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" s="4">
         <v>5</v>
@@ -1951,27 +1778,20 @@
       <c r="K36" s="4">
         <v>5</v>
       </c>
-      <c r="L36" s="4">
-        <v>5</v>
-      </c>
-      <c r="M36" s="6">
-        <v>5</v>
-      </c>
-      <c r="N36" s="2"/>
-      <c r="O36" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q36" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N36" s="4">
+        <v>5</v>
+      </c>
+      <c r="O36" s="6">
+        <v>5</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="4">
         <v>5</v>
@@ -1997,27 +1817,20 @@
       <c r="K37" s="4">
         <v>5</v>
       </c>
-      <c r="L37" s="4">
-        <v>5</v>
-      </c>
-      <c r="M37" s="6">
-        <v>5</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q37" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R37">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N37" s="4">
+        <v>5</v>
+      </c>
+      <c r="O37" s="6">
+        <v>5</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38" s="4">
         <v>5</v>
@@ -2043,27 +1856,20 @@
       <c r="K38" s="4">
         <v>5</v>
       </c>
-      <c r="L38" s="4">
-        <v>5</v>
-      </c>
-      <c r="M38" s="6">
-        <v>5</v>
-      </c>
-      <c r="N38" s="2"/>
-      <c r="O38" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q38" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N38" s="4">
+        <v>5</v>
+      </c>
+      <c r="O38" s="6">
+        <v>5</v>
+      </c>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:17" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="4">
         <v>5</v>
@@ -2089,94 +1895,44 @@
       <c r="K39" s="4">
         <v>5</v>
       </c>
-      <c r="L39" s="4">
-        <v>5</v>
-      </c>
-      <c r="M39" s="6">
-        <v>5</v>
-      </c>
-      <c r="N39" s="2"/>
-      <c r="O39" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q39" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R39">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="3:18" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D40" s="4">
-        <v>5</v>
-      </c>
-      <c r="E40" s="4">
-        <v>5</v>
-      </c>
-      <c r="F40" s="4">
-        <v>5</v>
-      </c>
-      <c r="G40" s="6">
-        <v>5</v>
-      </c>
-      <c r="H40" s="6">
-        <v>5</v>
-      </c>
-      <c r="I40" s="4">
-        <v>5</v>
-      </c>
-      <c r="J40" s="4">
-        <v>5</v>
-      </c>
-      <c r="K40" s="4">
-        <v>5</v>
-      </c>
-      <c r="L40" s="4">
-        <v>5</v>
-      </c>
-      <c r="M40" s="6">
-        <v>5</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q40" s="9">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="R40">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="3:18" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="N39" s="4">
+        <v>5</v>
+      </c>
+      <c r="O39" s="6">
+        <v>5</v>
+      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="3:17" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+    </row>
+    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-    </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">
@@ -2200,12 +1956,9 @@
     <row r="55" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H55" s="8"/>
     </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H56" s="8"/>
-    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="Q4:Q40 R25:R27 R29:R30">
+  <conditionalFormatting sqref="R24:R26 R28:R29">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2217,7 +1970,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R4:R31">
+  <conditionalFormatting sqref="R3:R30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 22:34:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -258,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,6 +298,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -605,10 +608,10 @@
   <dimension ref="A1:U55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T3" sqref="T3"/>
+      <selection pane="bottomRight" activeCell="U30" sqref="U30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -915,6 +918,9 @@
       <c r="T9" s="8">
         <v>5</v>
       </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1044,6 +1050,9 @@
       <c r="T13" s="8">
         <v>5</v>
       </c>
+      <c r="U13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1145,7 +1154,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:20" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1163,7 +1172,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:20" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1181,7 +1190,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1225,7 +1234,7 @@
       </c>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1260,8 +1269,11 @@
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="8"/>
-    </row>
-    <row r="21" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1303,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1336,7 +1348,7 @@
       </c>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1375,8 +1387,11 @@
       <c r="T23" s="15">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1427,8 +1442,11 @@
       <c r="T24" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U24" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1461,8 +1479,9 @@
       <c r="T25" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U25" s="8"/>
+    </row>
+    <row r="26" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1501,8 +1520,11 @@
       <c r="T26" s="16">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U26" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1556,8 +1578,11 @@
       <c r="T27" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U27" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1588,7 +1613,7 @@
       </c>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1620,7 +1645,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1674,8 +1699,11 @@
       <c r="T30" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U30" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1691,7 +1719,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 8:46:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Алигишиев Ибрагим</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>Лаб7</t>
+  </si>
+  <si>
+    <t>Лаб8</t>
+  </si>
+  <si>
+    <t>Лаб9</t>
   </si>
 </sst>
 </file>
@@ -605,13 +611,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U55"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="U30" sqref="U30"/>
+      <selection pane="bottomRight" activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -626,7 +632,7 @@
     <col min="19" max="21" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
@@ -681,8 +687,14 @@
       <c r="U1" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -696,7 +708,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(B3=C3,A2+1,"-------------------")</f>
         <v>1</v>
@@ -726,7 +738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="0">IF(B4=C4,A3+1,"-------------------")</f>
         <v>2</v>
@@ -755,7 +767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -784,7 +796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -811,7 +823,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -843,7 +855,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -876,7 +888,7 @@
       </c>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -922,7 +934,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -952,7 +964,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -983,7 +995,7 @@
       </c>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1013,7 +1025,7 @@
       </c>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1054,7 +1066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1084,7 +1096,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1118,7 +1130,7 @@
       </c>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1154,7 +1166,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1172,7 +1184,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:21" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1190,7 +1202,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1234,7 +1246,7 @@
       </c>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1273,7 +1285,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1314,8 +1326,11 @@
       <c r="T21" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1348,7 +1363,7 @@
       </c>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1390,8 +1405,14 @@
       <c r="U23" s="17">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V23">
+        <v>5</v>
+      </c>
+      <c r="W23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1446,7 +1467,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1481,7 +1502,7 @@
       </c>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1524,7 +1545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1581,8 +1602,11 @@
       <c r="U27" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1613,7 +1637,7 @@
       </c>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1645,7 +1669,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1702,8 +1726,11 @@
       <c r="U30" s="14">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1719,7 +1746,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 8:48:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
   <si>
     <t>Алигишиев Ибрагим</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Лаб9</t>
+  </si>
+  <si>
+    <t>Лаб10</t>
   </si>
 </sst>
 </file>
@@ -611,13 +614,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W31" sqref="W31"/>
+      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -632,7 +635,7 @@
     <col min="19" max="21" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
@@ -693,8 +696,11 @@
       <c r="W1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -708,7 +714,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
     </row>
-    <row r="3" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(B3=C3,A2+1,"-------------------")</f>
         <v>1</v>
@@ -738,7 +744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="0">IF(B4=C4,A3+1,"-------------------")</f>
         <v>2</v>
@@ -767,7 +773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -796,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -823,7 +829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -855,7 +861,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -888,7 +894,7 @@
       </c>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -934,7 +940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -964,7 +970,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -995,7 +1001,7 @@
       </c>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1025,7 +1031,7 @@
       </c>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1066,7 +1072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1096,7 +1102,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1130,7 +1136,7 @@
       </c>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1166,7 +1172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1184,7 +1190,7 @@
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
     </row>
-    <row r="18" spans="1:23" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1202,7 +1208,7 @@
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
     </row>
-    <row r="19" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1246,7 +1252,7 @@
       </c>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1285,7 +1291,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1329,8 +1335,11 @@
       <c r="W21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1363,7 +1372,7 @@
       </c>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1411,8 +1420,11 @@
       <c r="W23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1467,7 +1479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1502,7 +1514,7 @@
       </c>
       <c r="U25" s="8"/>
     </row>
-    <row r="26" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1545,7 +1557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1606,7 +1618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1637,7 +1649,7 @@
       </c>
       <c r="T28" s="16"/>
     </row>
-    <row r="29" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1669,7 +1681,7 @@
       <c r="S29" s="2"/>
       <c r="T29" s="16"/>
     </row>
-    <row r="30" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1730,7 +1742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1746,7 +1758,7 @@
       <c r="S31" s="4"/>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:23" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 8:52:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -617,10 +617,10 @@
   <dimension ref="A1:X55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
+      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1617,6 +1617,9 @@
       <c r="W27">
         <v>5</v>
       </c>
+      <c r="X27">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
@@ -1739,6 +1742,9 @@
         <v>5</v>
       </c>
       <c r="W30">
+        <v>5</v>
+      </c>
+      <c r="X30">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 8:59:51_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>Алигишиев Ибрагим</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t>Лаб10</t>
+  </si>
+  <si>
+    <t>Лаб11</t>
+  </si>
+  <si>
+    <t>Тест</t>
   </si>
 </sst>
 </file>
@@ -267,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -308,6 +314,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -614,13 +623,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X55"/>
+  <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X30" sqref="X30"/>
+      <selection pane="bottomRight" activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -635,7 +644,7 @@
     <col min="19" max="21" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
@@ -672,35 +681,41 @@
       <c r="O1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -709,12 +724,12 @@
       <c r="H2" s="3"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="3"/>
       <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(B3=C3,A2+1,"-------------------")</f>
         <v>1</v>
@@ -736,15 +751,15 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
-      <c r="P3" s="4">
-        <v>5</v>
-      </c>
-      <c r="R3" s="2"/>
-      <c r="S3" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q3" s="4">
+        <v>5</v>
+      </c>
+      <c r="S3" s="2"/>
+      <c r="T3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="0">IF(B4=C4,A3+1,"-------------------")</f>
         <v>2</v>
@@ -765,15 +780,15 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
-      <c r="P4" s="4">
-        <v>5</v>
-      </c>
-      <c r="R4" s="2"/>
-      <c r="S4" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q4" s="4">
+        <v>5</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -794,15 +809,15 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="P5" s="4">
-        <v>5</v>
-      </c>
-      <c r="R5" s="2"/>
-      <c r="S5" s="4">
+      <c r="Q5" s="4">
+        <v>5</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -821,15 +836,15 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-      <c r="P6" s="4">
-        <v>5</v>
-      </c>
-      <c r="R6" s="2"/>
-      <c r="S6" s="4">
+      <c r="Q6" s="4">
+        <v>5</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -854,14 +869,20 @@
       <c r="O7">
         <v>5</v>
       </c>
-      <c r="P7" s="4">
-        <v>5</v>
-      </c>
-      <c r="R7" s="2"/>
+      <c r="P7">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>5</v>
+      </c>
       <c r="S7" s="2"/>
-      <c r="T7" s="8"/>
-    </row>
-    <row r="8" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T7" s="2"/>
+      <c r="U7" s="8"/>
+      <c r="Z7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -882,19 +903,19 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-      <c r="P8" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>5</v>
-      </c>
-      <c r="R8" s="2"/>
-      <c r="S8" s="4">
-        <v>5</v>
-      </c>
-      <c r="T8" s="8"/>
-    </row>
-    <row r="9" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q8" s="4">
+        <v>5</v>
+      </c>
+      <c r="R8" s="5">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="4">
+        <v>5</v>
+      </c>
+      <c r="U8" s="8"/>
+    </row>
+    <row r="9" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -926,21 +947,24 @@
       <c r="M9" s="13">
         <v>5</v>
       </c>
-      <c r="P9" s="4">
-        <v>5</v>
-      </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="4">
-        <v>5</v>
-      </c>
-      <c r="T9" s="8">
-        <v>5</v>
-      </c>
-      <c r="U9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P9">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>5</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="4">
+        <v>5</v>
+      </c>
+      <c r="U9" s="8">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -963,14 +987,14 @@
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-      <c r="P10" s="4">
-        <v>5</v>
-      </c>
-      <c r="R10" s="2"/>
+      <c r="Q10" s="4">
+        <v>5</v>
+      </c>
       <c r="S10" s="2"/>
-      <c r="T10" s="8"/>
-    </row>
-    <row r="11" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T10" s="2"/>
+      <c r="U10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -992,16 +1016,16 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="P11" s="4">
-        <v>5</v>
-      </c>
-      <c r="R11" s="2"/>
-      <c r="S11" s="4">
-        <v>5</v>
-      </c>
-      <c r="T11" s="8"/>
-    </row>
-    <row r="12" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q11" s="4">
+        <v>5</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="4">
+        <v>5</v>
+      </c>
+      <c r="U11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1024,14 +1048,14 @@
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="P12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="4">
-        <v>5</v>
-      </c>
-      <c r="T12" s="8"/>
-    </row>
-    <row r="13" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="4">
+        <v>5</v>
+      </c>
+      <c r="U12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1057,22 +1081,22 @@
       <c r="M13">
         <v>5</v>
       </c>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="5">
-        <v>5</v>
-      </c>
-      <c r="R13" s="2"/>
-      <c r="S13" s="4">
-        <v>5</v>
-      </c>
-      <c r="T13" s="8">
-        <v>5</v>
-      </c>
-      <c r="U13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="2"/>
+      <c r="R13" s="5">
+        <v>5</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="4">
+        <v>5</v>
+      </c>
+      <c r="U13" s="8">
+        <v>5</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1095,14 +1119,14 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="P14" s="4">
-        <v>5</v>
-      </c>
-      <c r="R14" s="2"/>
+      <c r="Q14" s="4">
+        <v>5</v>
+      </c>
       <c r="S14" s="2"/>
-      <c r="T14" s="8"/>
-    </row>
-    <row r="15" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T14" s="2"/>
+      <c r="U14" s="8"/>
+    </row>
+    <row r="15" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1127,16 +1151,16 @@
       <c r="K15" s="8">
         <v>5</v>
       </c>
-      <c r="P15" s="4">
-        <v>5</v>
-      </c>
-      <c r="R15" s="2"/>
-      <c r="S15" s="4">
+      <c r="Q15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="T15" s="4">
         <v>4</v>
       </c>
-      <c r="T15" s="8"/>
-    </row>
-    <row r="16" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U15" s="8"/>
+    </row>
+    <row r="16" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1161,18 +1185,18 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="P16" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="5">
-        <v>5</v>
-      </c>
-      <c r="R16" s="2"/>
-      <c r="S16" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="4">
+        <v>5</v>
+      </c>
+      <c r="R16" s="5">
+        <v>5</v>
+      </c>
+      <c r="S16" s="2"/>
+      <c r="T16" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1186,11 +1210,11 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="R17" s="12"/>
+      <c r="Q17" s="12"/>
       <c r="S17" s="12"/>
-    </row>
-    <row r="18" spans="1:24" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T17" s="12"/>
+    </row>
+    <row r="18" spans="1:26" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1204,11 +1228,11 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="R18" s="12"/>
+      <c r="Q18" s="12"/>
       <c r="S18" s="12"/>
-    </row>
-    <row r="19" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T18" s="12"/>
+    </row>
+    <row r="19" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1240,19 +1264,22 @@
       <c r="K19" s="4">
         <v>5</v>
       </c>
-      <c r="P19" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>5</v>
-      </c>
-      <c r="R19" s="2"/>
-      <c r="S19" s="4">
-        <v>5</v>
-      </c>
-      <c r="T19" s="8"/>
-    </row>
-    <row r="20" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P19">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>5</v>
+      </c>
+      <c r="R19" s="7">
+        <v>5</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="4">
+        <v>5</v>
+      </c>
+      <c r="U19" s="8"/>
+    </row>
+    <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1281,17 +1308,17 @@
       <c r="O20">
         <v>5</v>
       </c>
-      <c r="P20" s="4">
-        <v>5</v>
-      </c>
-      <c r="R20" s="2"/>
+      <c r="Q20" s="4">
+        <v>5</v>
+      </c>
       <c r="S20" s="2"/>
-      <c r="T20" s="8"/>
-      <c r="U20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T20" s="2"/>
+      <c r="U20" s="8"/>
+      <c r="V20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1322,24 +1349,24 @@
       <c r="O21">
         <v>5</v>
       </c>
-      <c r="P21" s="4">
-        <v>5</v>
-      </c>
-      <c r="R21" s="2"/>
-      <c r="S21" s="4">
-        <v>5</v>
-      </c>
-      <c r="T21" s="8">
-        <v>5</v>
-      </c>
-      <c r="W21">
+      <c r="Q21" s="4">
+        <v>5</v>
+      </c>
+      <c r="S21" s="2"/>
+      <c r="T21" s="4">
+        <v>5</v>
+      </c>
+      <c r="U21" s="8">
         <v>5</v>
       </c>
       <c r="X21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1360,19 +1387,19 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="P22" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q22" s="5">
-        <v>5</v>
-      </c>
-      <c r="R22" s="2"/>
-      <c r="S22" s="4">
-        <v>5</v>
-      </c>
-      <c r="T22" s="8"/>
-    </row>
-    <row r="23" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q22" s="4">
+        <v>5</v>
+      </c>
+      <c r="R22" s="5">
+        <v>5</v>
+      </c>
+      <c r="S22" s="2"/>
+      <c r="T22" s="4">
+        <v>5</v>
+      </c>
+      <c r="U22" s="8"/>
+    </row>
+    <row r="23" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1396,25 +1423,25 @@
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-      <c r="P23" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q23" s="5">
-        <v>5</v>
-      </c>
-      <c r="R23" s="4">
+      <c r="P23">
+        <v>5</v>
+      </c>
+      <c r="Q23" s="4">
+        <v>5</v>
+      </c>
+      <c r="R23" s="5">
         <v>5</v>
       </c>
       <c r="S23" s="4">
         <v>5</v>
       </c>
-      <c r="T23" s="15">
-        <v>5</v>
-      </c>
-      <c r="U23" s="17">
-        <v>5</v>
-      </c>
-      <c r="V23">
+      <c r="T23" s="4">
+        <v>5</v>
+      </c>
+      <c r="U23" s="15">
+        <v>5</v>
+      </c>
+      <c r="V23" s="17">
         <v>5</v>
       </c>
       <c r="W23">
@@ -1423,8 +1450,11 @@
       <c r="X23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1460,7 +1490,7 @@
       <c r="M24" s="14">
         <v>5</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24">
         <v>5</v>
       </c>
       <c r="Q24" s="4">
@@ -1472,14 +1502,17 @@
       <c r="S24" s="4">
         <v>5</v>
       </c>
-      <c r="T24" s="16">
-        <v>5</v>
-      </c>
-      <c r="U24" s="14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="T24" s="4">
+        <v>5</v>
+      </c>
+      <c r="U24" s="16">
+        <v>5</v>
+      </c>
+      <c r="V24" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1502,19 +1535,19 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="P25" s="4">
-        <v>5</v>
-      </c>
-      <c r="R25" s="2"/>
-      <c r="S25" s="4">
-        <v>5</v>
-      </c>
-      <c r="T25" s="16">
+      <c r="Q25" s="4">
+        <v>5</v>
+      </c>
+      <c r="S25" s="2"/>
+      <c r="T25" s="4">
+        <v>5</v>
+      </c>
+      <c r="U25" s="16">
         <v>3</v>
       </c>
-      <c r="U25" s="8"/>
-    </row>
-    <row r="26" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="8"/>
+    </row>
+    <row r="26" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1540,24 +1573,24 @@
       <c r="M26">
         <v>5</v>
       </c>
-      <c r="P26" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="5">
-        <v>5</v>
-      </c>
-      <c r="R26" s="2"/>
-      <c r="S26" s="4">
-        <v>5</v>
-      </c>
-      <c r="T26" s="16">
-        <v>5</v>
-      </c>
-      <c r="U26" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q26" s="4">
+        <v>5</v>
+      </c>
+      <c r="R26" s="5">
+        <v>5</v>
+      </c>
+      <c r="S26" s="2"/>
+      <c r="T26" s="4">
+        <v>5</v>
+      </c>
+      <c r="U26" s="16">
+        <v>5</v>
+      </c>
+      <c r="V26" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1598,30 +1631,36 @@
       <c r="N27" s="13">
         <v>5</v>
       </c>
-      <c r="P27" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q27" s="5">
-        <v>5</v>
-      </c>
-      <c r="R27" s="2"/>
-      <c r="S27" s="4">
-        <v>5</v>
-      </c>
-      <c r="T27" s="8">
+      <c r="P27">
+        <v>5</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>5</v>
+      </c>
+      <c r="R27" s="5">
+        <v>5</v>
+      </c>
+      <c r="S27" s="2"/>
+      <c r="T27" s="4">
         <v>5</v>
       </c>
       <c r="U27" s="8">
         <v>5</v>
       </c>
-      <c r="W27">
+      <c r="V27" s="8">
         <v>5</v>
       </c>
       <c r="X27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y27">
+        <v>5</v>
+      </c>
+      <c r="Z27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1643,16 +1682,19 @@
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="N28" s="8"/>
-      <c r="P28" s="4">
-        <v>5</v>
-      </c>
-      <c r="R28" s="2"/>
-      <c r="S28" s="4">
-        <v>5</v>
-      </c>
-      <c r="T28" s="16"/>
-    </row>
-    <row r="29" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P28">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>5</v>
+      </c>
+      <c r="S28" s="2"/>
+      <c r="T28" s="4">
+        <v>5</v>
+      </c>
+      <c r="U28" s="16"/>
+    </row>
+    <row r="29" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1675,16 +1717,16 @@
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="N29" s="8"/>
-      <c r="P29" s="4">
-        <v>5</v>
-      </c>
-      <c r="R29" s="4">
-        <v>5</v>
-      </c>
-      <c r="S29" s="2"/>
-      <c r="T29" s="16"/>
-    </row>
-    <row r="30" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q29" s="4">
+        <v>5</v>
+      </c>
+      <c r="S29" s="4">
+        <v>5</v>
+      </c>
+      <c r="T29" s="2"/>
+      <c r="U29" s="16"/>
+    </row>
+    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1725,30 +1767,36 @@
       <c r="O30">
         <v>5</v>
       </c>
-      <c r="P30" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>5</v>
-      </c>
-      <c r="R30" s="2"/>
-      <c r="S30" s="4">
-        <v>5</v>
-      </c>
-      <c r="T30" s="8">
-        <v>5</v>
-      </c>
-      <c r="U30" s="14">
-        <v>5</v>
-      </c>
-      <c r="W30">
+      <c r="P30">
+        <v>5</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>5</v>
+      </c>
+      <c r="R30" s="6">
+        <v>5</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="4">
+        <v>5</v>
+      </c>
+      <c r="U30" s="8">
+        <v>5</v>
+      </c>
+      <c r="V30" s="14">
         <v>5</v>
       </c>
       <c r="X30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y30">
+        <v>5</v>
+      </c>
+      <c r="Z30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1758,13 +1806,13 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="4"/>
-      <c r="T31" s="8"/>
-    </row>
-    <row r="32" spans="1:24" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q31" s="4"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="4"/>
+      <c r="U31" s="8"/>
+    </row>
+    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1774,12 +1822,12 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="4"/>
-    </row>
-    <row r="33" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q32" s="4"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="4"/>
+    </row>
+    <row r="33" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -1789,12 +1837,12 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="P33" s="4"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="4"/>
-    </row>
-    <row r="34" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="4"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -1804,12 +1852,12 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="2"/>
-      <c r="S34" s="4"/>
-    </row>
-    <row r="35" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="4"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="4"/>
+    </row>
+    <row r="35" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -1819,12 +1867,12 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="2"/>
-      <c r="S35" s="4"/>
-    </row>
-    <row r="36" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="4"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="4"/>
+    </row>
+    <row r="36" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -1834,12 +1882,12 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="P36" s="4"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="2"/>
-      <c r="S36" s="4"/>
-    </row>
-    <row r="37" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="4"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="4"/>
+    </row>
+    <row r="37" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -1849,12 +1897,12 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="4"/>
-    </row>
-    <row r="38" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q37" s="4"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="2"/>
+      <c r="T37" s="4"/>
+    </row>
+    <row r="38" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -1864,12 +1912,12 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="P38" s="4"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="2"/>
-      <c r="S38" s="4"/>
-    </row>
-    <row r="39" spans="3:19" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q38" s="4"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -1879,38 +1927,38 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="2"/>
-      <c r="S39" s="4"/>
-    </row>
-    <row r="40" spans="3:19" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Q39" s="4"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="3:20" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:04:11_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -626,10 +626,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P30" sqref="P30"/>
+      <selection pane="bottomRight" activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1511,6 +1511,9 @@
       <c r="V24" s="14">
         <v>5</v>
       </c>
+      <c r="X24">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
@@ -1587,6 +1590,9 @@
         <v>5</v>
       </c>
       <c r="V26" s="8">
+        <v>5</v>
+      </c>
+      <c r="X26">
         <v>5</v>
       </c>
     </row>
@@ -1725,6 +1731,9 @@
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="16"/>
+      <c r="X29">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:08:59_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -273,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -317,6 +317,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,10 +629,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="K11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Y24" sqref="Y24"/>
+      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1081,6 +1084,9 @@
       <c r="M13">
         <v>5</v>
       </c>
+      <c r="P13">
+        <v>5</v>
+      </c>
       <c r="Q13" s="2"/>
       <c r="R13" s="5">
         <v>5</v>
@@ -1093,6 +1099,9 @@
         <v>5</v>
       </c>
       <c r="V13">
+        <v>5</v>
+      </c>
+      <c r="X13">
         <v>5</v>
       </c>
     </row>
@@ -1511,6 +1520,9 @@
       <c r="V24" s="14">
         <v>5</v>
       </c>
+      <c r="W24" s="19">
+        <v>5</v>
+      </c>
       <c r="X24">
         <v>5</v>
       </c>
@@ -1590,6 +1602,9 @@
         <v>5</v>
       </c>
       <c r="V26" s="8">
+        <v>5</v>
+      </c>
+      <c r="W26">
         <v>5</v>
       </c>
       <c r="X26">
@@ -1731,6 +1746,9 @@
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="16"/>
+      <c r="W29">
+        <v>5</v>
+      </c>
       <c r="X29">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:14:25_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -629,10 +629,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
+      <selection pane="bottomRight" activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1101,6 +1101,9 @@
       <c r="V13">
         <v>5</v>
       </c>
+      <c r="W13">
+        <v>5</v>
+      </c>
       <c r="X13">
         <v>5</v>
       </c>
@@ -1287,6 +1290,9 @@
         <v>5</v>
       </c>
       <c r="U19" s="8"/>
+      <c r="V19" s="19">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -1746,6 +1752,9 @@
       </c>
       <c r="T29" s="2"/>
       <c r="U29" s="16"/>
+      <c r="V29" s="16">
+        <v>5</v>
+      </c>
       <c r="W29">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:21:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -629,10 +629,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="V19" sqref="V19"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1084,6 +1084,12 @@
       <c r="M13">
         <v>5</v>
       </c>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13">
+        <v>5</v>
+      </c>
       <c r="P13">
         <v>5</v>
       </c>
@@ -1289,7 +1295,9 @@
       <c r="T19" s="4">
         <v>5</v>
       </c>
-      <c r="U19" s="8"/>
+      <c r="U19" s="8">
+        <v>5</v>
+      </c>
       <c r="V19" s="19">
         <v>5</v>
       </c>
@@ -1435,9 +1443,15 @@
       <c r="G23" s="5">
         <v>5</v>
       </c>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="I23" s="8">
+        <v>5</v>
+      </c>
+      <c r="J23" s="8">
+        <v>5</v>
+      </c>
+      <c r="K23" s="8">
+        <v>5</v>
+      </c>
       <c r="P23">
         <v>5</v>
       </c>
@@ -1503,6 +1517,12 @@
         <v>5</v>
       </c>
       <c r="M24" s="14">
+        <v>5</v>
+      </c>
+      <c r="N24" s="19">
+        <v>5</v>
+      </c>
+      <c r="O24">
         <v>5</v>
       </c>
       <c r="P24">
@@ -1594,6 +1614,12 @@
       <c r="M26">
         <v>5</v>
       </c>
+      <c r="N26">
+        <v>5</v>
+      </c>
+      <c r="O26">
+        <v>5</v>
+      </c>
       <c r="Q26" s="4">
         <v>5</v>
       </c>
@@ -1708,7 +1734,9 @@
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-      <c r="N28" s="8"/>
+      <c r="N28" s="8">
+        <v>5</v>
+      </c>
       <c r="P28">
         <v>5</v>
       </c>
@@ -1743,7 +1771,12 @@
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="N29" s="8"/>
+      <c r="N29" s="8">
+        <v>5</v>
+      </c>
+      <c r="O29">
+        <v>5</v>
+      </c>
       <c r="Q29" s="4">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_16 июня 2024 г. 13:29:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -629,10 +629,10 @@
   <dimension ref="A1:Z55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="I11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I23" sqref="I23"/>
+      <selection pane="bottomRight" activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1439,8 +1439,13 @@
       <c r="E23" s="4">
         <v>5</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
       <c r="G23" s="5">
+        <v>5</v>
+      </c>
+      <c r="H23">
         <v>5</v>
       </c>
       <c r="I23" s="8">
@@ -1618,6 +1623,9 @@
         <v>5</v>
       </c>
       <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
         <v>5</v>
       </c>
       <c r="Q26" s="4">

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 9:27:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -632,10 +632,10 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="X12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AD16" sqref="AD16"/>
+      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -796,6 +796,9 @@
       <c r="T4" s="4">
         <v>5</v>
       </c>
+      <c r="AD4">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -923,6 +926,9 @@
         <v>5</v>
       </c>
       <c r="U8" s="8"/>
+      <c r="AD8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -971,6 +977,9 @@
       </c>
       <c r="V9">
         <v>5</v>
+      </c>
+      <c r="AD9">
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1063,6 +1072,9 @@
         <v>5</v>
       </c>
       <c r="U12" s="8"/>
+      <c r="AD12">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1220,7 +1232,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:26" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1238,7 +1250,7 @@
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
     </row>
-    <row r="18" spans="1:26" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1256,7 +1268,7 @@
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
     </row>
-    <row r="19" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1308,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1347,7 +1359,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1394,8 +1406,11 @@
       <c r="Y21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1428,7 +1443,7 @@
       </c>
       <c r="U22" s="8"/>
     </row>
-    <row r="23" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1493,8 +1508,11 @@
       <c r="Y23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1564,7 +1582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1599,7 +1617,7 @@
       </c>
       <c r="V25" s="8"/>
     </row>
-    <row r="26" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1656,8 +1674,11 @@
       <c r="X26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1727,7 +1748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1762,8 +1783,11 @@
         <v>5</v>
       </c>
       <c r="U28" s="16"/>
-    </row>
-    <row r="29" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1809,7 +1833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1879,7 +1903,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1895,7 +1919,7 @@
       <c r="T31" s="4"/>
       <c r="U31" s="8"/>
     </row>
-    <row r="32" spans="1:26" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 9:30:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Алигишиев Ибрагим</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Вариант</t>
+  </si>
+  <si>
+    <t>оценко</t>
   </si>
 </sst>
 </file>
@@ -629,13 +632,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD55"/>
+  <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AD5" sqref="AD5"/>
+      <selection pane="bottomRight" activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -650,7 +653,7 @@
     <col min="19" max="21" width="5.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="29" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
@@ -723,8 +726,11 @@
       <c r="AD1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -738,7 +744,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <f>IF(B3=C3,A2+1,"-------------------")</f>
         <v>1</v>
@@ -768,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <f t="shared" ref="A4:A30" si="0">IF(B4=C4,A3+1,"-------------------")</f>
         <v>2</v>
@@ -800,7 +806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -829,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -856,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -894,7 +900,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -929,8 +935,11 @@
       <c r="AD8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -982,7 +991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1012,7 +1021,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="8"/>
     </row>
-    <row r="11" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1043,7 +1052,7 @@
       </c>
       <c r="U11" s="8"/>
     </row>
-    <row r="12" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1076,7 +1085,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1132,7 +1141,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1162,7 +1171,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="8"/>
     </row>
-    <row r="15" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1196,7 +1205,7 @@
       </c>
       <c r="U15" s="8"/>
     </row>
-    <row r="16" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>14</v>

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 9:31:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="R9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE8" sqref="AE8"/>
+      <selection pane="bottomRight" activeCell="AD28" sqref="AD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1756,6 +1756,9 @@
       <c r="Z27">
         <v>5</v>
       </c>
+      <c r="AD27">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 11:31:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="S6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AD28" sqref="AD28"/>
+      <selection pane="bottomRight" activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -805,6 +805,9 @@
       <c r="AD4">
         <v>9</v>
       </c>
+      <c r="AE4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -861,6 +864,9 @@
       <c r="T6" s="4">
         <v>4</v>
       </c>
+      <c r="AD6">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -898,6 +904,9 @@
       <c r="U7" s="8"/>
       <c r="Z7">
         <v>5</v>
+      </c>
+      <c r="AD7">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -990,6 +999,9 @@
       <c r="AD9">
         <v>13</v>
       </c>
+      <c r="AE9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -1020,6 +1032,9 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="8"/>
+      <c r="AD10">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -1084,6 +1099,9 @@
       <c r="AD12">
         <v>24</v>
       </c>
+      <c r="AE12">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -1140,6 +1158,9 @@
       <c r="X13">
         <v>5</v>
       </c>
+      <c r="AD13">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -1170,6 +1191,9 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="8"/>
+      <c r="AD14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1204,6 +1228,9 @@
         <v>4</v>
       </c>
       <c r="U15" s="8"/>
+      <c r="AD15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -1240,8 +1267,14 @@
       <c r="T16" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:30" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD16">
+        <v>27</v>
+      </c>
+      <c r="AE16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1259,7 +1292,7 @@
       <c r="S17" s="12"/>
       <c r="T17" s="12"/>
     </row>
-    <row r="18" spans="1:30" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1277,7 +1310,7 @@
       <c r="S18" s="12"/>
       <c r="T18" s="12"/>
     </row>
-    <row r="19" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1328,8 +1361,14 @@
       <c r="V19" s="19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD19">
+        <v>28</v>
+      </c>
+      <c r="AE19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1368,7 +1407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1418,8 +1457,11 @@
       <c r="AD21">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1451,8 +1493,11 @@
         <v>5</v>
       </c>
       <c r="U22" s="8"/>
-    </row>
-    <row r="23" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD22">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1520,8 +1565,11 @@
       <c r="AD23">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1590,8 +1638,11 @@
       <c r="X24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1625,8 +1676,14 @@
         <v>3</v>
       </c>
       <c r="V25" s="8"/>
-    </row>
-    <row r="26" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD25">
+        <v>22</v>
+      </c>
+      <c r="AE25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1684,10 +1741,13 @@
         <v>5</v>
       </c>
       <c r="AD26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="AE26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1759,8 +1819,11 @@
       <c r="AD27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1798,8 +1861,11 @@
       <c r="AD28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1844,8 +1910,11 @@
       <c r="X29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1914,8 +1983,14 @@
       <c r="Z30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AD30">
+        <v>18</v>
+      </c>
+      <c r="AE30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="1"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -1931,7 +2006,7 @@
       <c r="T31" s="4"/>
       <c r="U31" s="8"/>
     </row>
-    <row r="32" spans="1:30" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 11:34:30_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="S6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE16" sqref="AE16"/>
+      <selection pane="bottomRight" activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1161,6 +1161,9 @@
       <c r="AD13">
         <v>11</v>
       </c>
+      <c r="AE13">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 12:28:14_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="U6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE14" sqref="AE14"/>
+      <selection pane="bottomRight" activeCell="AE31" sqref="AE31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -773,6 +773,12 @@
       <c r="T3" s="4">
         <v>5</v>
       </c>
+      <c r="AD3">
+        <v>13</v>
+      </c>
+      <c r="AE3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -836,6 +842,12 @@
       <c r="S5" s="2"/>
       <c r="T5" s="4">
         <v>3</v>
+      </c>
+      <c r="AD5">
+        <v>14</v>
+      </c>
+      <c r="AE5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1066,6 +1078,12 @@
         <v>5</v>
       </c>
       <c r="U11" s="8"/>
+      <c r="AD11">
+        <v>15</v>
+      </c>
+      <c r="AE11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -1197,6 +1215,9 @@
       <c r="AD14">
         <v>3</v>
       </c>
+      <c r="AE14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -1233,6 +1254,9 @@
       <c r="U15" s="8"/>
       <c r="AD15">
         <v>5</v>
+      </c>
+      <c r="AE15">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1409,6 +1433,12 @@
       <c r="V20">
         <v>5</v>
       </c>
+      <c r="AD20">
+        <v>9</v>
+      </c>
+      <c r="AE20">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -1499,6 +1529,9 @@
       <c r="AD22">
         <v>12</v>
       </c>
+      <c r="AE22">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
@@ -1643,6 +1676,9 @@
       </c>
       <c r="AD24">
         <v>22</v>
+      </c>
+      <c r="AE24">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1915,6 +1951,9 @@
       </c>
       <c r="AD29">
         <v>13</v>
+      </c>
+      <c r="AE29">
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_22 июня 2024 г. 13:16:13_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="U19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE31" sqref="AE31"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -879,6 +879,9 @@
       <c r="AD6">
         <v>24</v>
       </c>
+      <c r="AE6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -919,6 +922,9 @@
       </c>
       <c r="AD7">
         <v>20</v>
+      </c>
+      <c r="AE7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1046,6 +1052,9 @@
       <c r="U10" s="8"/>
       <c r="AD10">
         <v>14</v>
+      </c>
+      <c r="AE10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_25 июня 2024 г. 9:23:54_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="U3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AC12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
+      <selection pane="bottomRight" activeCell="AE26" sqref="AE26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_25 июня 2024 г. 10:42:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="T8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AA1" sqref="AA1"/>
+      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -872,6 +872,9 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
+      <c r="P6">
+        <v>5</v>
+      </c>
       <c r="Q6" s="4">
         <v>5</v>
       </c>
@@ -1684,6 +1687,9 @@
         <v>5</v>
       </c>
       <c r="X24">
+        <v>5</v>
+      </c>
+      <c r="Z24">
         <v>5</v>
       </c>
       <c r="AD24">

</xml_diff>

<commit_message>
AutoCommit_28 июня 2024 г. 21:52:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Z24" sqref="Z24"/>
+      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -872,6 +872,15 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6">
+        <v>5</v>
+      </c>
       <c r="P6">
         <v>5</v>
       </c>
@@ -881,6 +890,15 @@
       <c r="S6" s="2"/>
       <c r="T6" s="4">
         <v>4</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>5</v>
+      </c>
+      <c r="Y6">
+        <v>5</v>
       </c>
       <c r="AD6">
         <v>24</v>
@@ -1250,6 +1268,9 @@
         <v>5</v>
       </c>
       <c r="F15" s="2"/>
+      <c r="H15">
+        <v>5</v>
+      </c>
       <c r="I15" s="8">
         <v>5</v>
       </c>
@@ -1259,14 +1280,40 @@
       <c r="K15" s="8">
         <v>5</v>
       </c>
+      <c r="M15" s="8">
+        <v>5</v>
+      </c>
+      <c r="N15" s="8">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>5</v>
+      </c>
       <c r="Q15" s="4">
+        <v>5</v>
+      </c>
+      <c r="R15">
         <v>5</v>
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="4">
         <v>4</v>
       </c>
-      <c r="U15" s="8"/>
+      <c r="U15" s="8">
+        <v>5</v>
+      </c>
+      <c r="V15">
+        <v>5</v>
+      </c>
+      <c r="X15">
+        <v>5</v>
+      </c>
+      <c r="Y15">
+        <v>5</v>
+      </c>
+      <c r="Z15">
+        <v>5</v>
+      </c>
       <c r="AD15">
         <v>5</v>
       </c>
@@ -1583,6 +1630,15 @@
       <c r="K23" s="8">
         <v>5</v>
       </c>
+      <c r="M23" s="8">
+        <v>5</v>
+      </c>
+      <c r="N23" s="8">
+        <v>5</v>
+      </c>
+      <c r="O23">
+        <v>5</v>
+      </c>
       <c r="P23">
         <v>5</v>
       </c>
@@ -1611,6 +1667,9 @@
         <v>5</v>
       </c>
       <c r="Y23">
+        <v>5</v>
+      </c>
+      <c r="Z23">
         <v>5</v>
       </c>
       <c r="AD23">
@@ -1687,6 +1746,9 @@
         <v>5</v>
       </c>
       <c r="X24">
+        <v>5</v>
+      </c>
+      <c r="Y24">
         <v>5</v>
       </c>
       <c r="Z24">
@@ -1914,7 +1976,15 @@
       <c r="T28" s="4">
         <v>5</v>
       </c>
-      <c r="U28" s="16"/>
+      <c r="U28" s="16">
+        <v>5</v>
+      </c>
+      <c r="V28" s="16">
+        <v>5</v>
+      </c>
+      <c r="X28">
+        <v>5</v>
+      </c>
       <c r="AD28">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 13:53:12_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -638,7 +638,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H15" sqref="H15"/>
+      <selection pane="bottomRight" activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -776,6 +776,15 @@
       <c r="T3" s="4">
         <v>5</v>
       </c>
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3">
+        <v>5</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
       <c r="AD3">
         <v>13</v>
       </c>
@@ -809,6 +818,15 @@
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="4">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="Y4">
+        <v>5</v>
+      </c>
+      <c r="Z4">
         <v>5</v>
       </c>
       <c r="AD4">
@@ -897,6 +915,9 @@
       <c r="W6">
         <v>5</v>
       </c>
+      <c r="X6">
+        <v>5</v>
+      </c>
       <c r="Y6">
         <v>5</v>
       </c>
@@ -983,6 +1004,15 @@
         <v>5</v>
       </c>
       <c r="U8" s="8"/>
+      <c r="X8">
+        <v>5</v>
+      </c>
+      <c r="Y8">
+        <v>5</v>
+      </c>
+      <c r="Z8">
+        <v>5</v>
+      </c>
       <c r="AD8">
         <v>7</v>
       </c>
@@ -1036,6 +1066,15 @@
         <v>5</v>
       </c>
       <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <v>5</v>
+      </c>
+      <c r="Y9">
+        <v>5</v>
+      </c>
+      <c r="Z9">
         <v>5</v>
       </c>
       <c r="AD9">
@@ -1111,6 +1150,12 @@
         <v>5</v>
       </c>
       <c r="U11" s="8"/>
+      <c r="X11">
+        <v>5</v>
+      </c>
+      <c r="Z11">
+        <v>5</v>
+      </c>
       <c r="AD11">
         <v>15</v>
       </c>
@@ -1207,6 +1252,12 @@
         <v>5</v>
       </c>
       <c r="X13">
+        <v>5</v>
+      </c>
+      <c r="Y13">
+        <v>5</v>
+      </c>
+      <c r="Z13">
         <v>5</v>
       </c>
       <c r="AD13">
@@ -1495,6 +1546,15 @@
       <c r="V20">
         <v>5</v>
       </c>
+      <c r="X20">
+        <v>5</v>
+      </c>
+      <c r="Y20">
+        <v>5</v>
+      </c>
+      <c r="Z20">
+        <v>5</v>
+      </c>
       <c r="AD20">
         <v>9</v>
       </c>
@@ -1795,6 +1855,15 @@
         <v>3</v>
       </c>
       <c r="V25" s="8"/>
+      <c r="X25">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>5</v>
+      </c>
+      <c r="Z25">
+        <v>5</v>
+      </c>
       <c r="AD25">
         <v>22</v>
       </c>
@@ -1857,6 +1926,12 @@
         <v>5</v>
       </c>
       <c r="X26">
+        <v>5</v>
+      </c>
+      <c r="Y26">
+        <v>5</v>
+      </c>
+      <c r="Z26">
         <v>5</v>
       </c>
       <c r="AD26">

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 13:54:11_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomRight" activeCell="W9" sqref="W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1004,6 +1004,9 @@
         <v>5</v>
       </c>
       <c r="U8" s="8"/>
+      <c r="W8">
+        <v>5</v>
+      </c>
       <c r="X8">
         <v>5</v>
       </c>
@@ -1066,6 +1069,9 @@
         <v>5</v>
       </c>
       <c r="V9">
+        <v>5</v>
+      </c>
+      <c r="W9">
         <v>5</v>
       </c>
       <c r="X9">
@@ -1546,6 +1552,9 @@
       <c r="V20">
         <v>5</v>
       </c>
+      <c r="W20">
+        <v>5</v>
+      </c>
       <c r="X20">
         <v>5</v>
       </c>
@@ -1855,6 +1864,9 @@
         <v>3</v>
       </c>
       <c r="V25" s="8"/>
+      <c r="W25">
+        <v>5</v>
+      </c>
       <c r="X25">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 14:01:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="W9" sqref="W9"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -769,11 +769,20 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
+      <c r="O3">
+        <v>5</v>
+      </c>
       <c r="Q3" s="4">
+        <v>5</v>
+      </c>
+      <c r="R3">
         <v>5</v>
       </c>
       <c r="S3" s="2"/>
       <c r="T3" s="4">
+        <v>5</v>
+      </c>
+      <c r="V3">
         <v>5</v>
       </c>
       <c r="X3">
@@ -813,11 +822,23 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
+      <c r="O4">
+        <v>5</v>
+      </c>
       <c r="Q4" s="4">
+        <v>5</v>
+      </c>
+      <c r="R4">
         <v>5</v>
       </c>
       <c r="S4" s="2"/>
       <c r="T4" s="4">
+        <v>5</v>
+      </c>
+      <c r="U4">
+        <v>5</v>
+      </c>
+      <c r="V4">
         <v>5</v>
       </c>
       <c r="X4">
@@ -993,6 +1014,12 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
       <c r="Q8" s="4">
         <v>5</v>
       </c>
@@ -1003,7 +1030,12 @@
       <c r="T8" s="4">
         <v>5</v>
       </c>
-      <c r="U8" s="8"/>
+      <c r="U8" s="8">
+        <v>5</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
       <c r="W8">
         <v>5</v>
       </c>
@@ -1053,6 +1085,12 @@
         <v>5</v>
       </c>
       <c r="M9" s="13">
+        <v>5</v>
+      </c>
+      <c r="N9" s="7">
+        <v>5</v>
+      </c>
+      <c r="O9">
         <v>5</v>
       </c>
       <c r="P9">
@@ -1148,14 +1186,28 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>5</v>
+      </c>
       <c r="Q11" s="4">
+        <v>5</v>
+      </c>
+      <c r="R11">
         <v>5</v>
       </c>
       <c r="S11" s="2"/>
       <c r="T11" s="4">
         <v>5</v>
       </c>
-      <c r="U11" s="8"/>
+      <c r="U11" s="8">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <v>5</v>
+      </c>
       <c r="X11">
         <v>5</v>
       </c>
@@ -1546,9 +1598,16 @@
       <c r="Q20" s="4">
         <v>5</v>
       </c>
+      <c r="R20">
+        <v>5</v>
+      </c>
       <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="8"/>
+      <c r="T20" s="2">
+        <v>5</v>
+      </c>
+      <c r="U20" s="8">
+        <v>5</v>
+      </c>
       <c r="V20">
         <v>5</v>
       </c>
@@ -1853,6 +1912,15 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
+      <c r="N25">
+        <v>5</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
+      </c>
+      <c r="P25">
+        <v>5</v>
+      </c>
       <c r="Q25" s="4">
         <v>5</v>
       </c>
@@ -1861,9 +1929,11 @@
         <v>5</v>
       </c>
       <c r="U25" s="16">
-        <v>3</v>
-      </c>
-      <c r="V25" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="V25" s="8">
+        <v>5</v>
+      </c>
       <c r="W25">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 14:45:49_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -638,7 +638,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -769,6 +769,12 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
       <c r="O3">
         <v>5</v>
       </c>
@@ -822,6 +828,12 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
       <c r="O4">
         <v>5</v>
       </c>
@@ -971,6 +983,12 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
+      <c r="M7">
+        <v>5</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
       <c r="O7">
         <v>5</v>
       </c>
@@ -1014,6 +1032,9 @@
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
+      <c r="M8">
+        <v>5</v>
+      </c>
       <c r="N8">
         <v>5</v>
       </c>
@@ -1186,6 +1207,9 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
+      <c r="M11">
+        <v>5</v>
+      </c>
       <c r="N11">
         <v>5</v>
       </c>
@@ -1589,6 +1613,9 @@
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
+      <c r="M20">
+        <v>5</v>
+      </c>
       <c r="N20">
         <v>5</v>
       </c>
@@ -1912,6 +1939,9 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
+      <c r="M25">
+        <v>5</v>
+      </c>
       <c r="N25">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 14:54:08_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -825,6 +825,9 @@
       <c r="F4" s="4">
         <v>5</v>
       </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
@@ -972,17 +975,30 @@
       <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
       <c r="E7" s="4">
         <v>5</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
       <c r="G7" s="5">
         <v>5</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="8">
+        <v>5</v>
+      </c>
+      <c r="J7" s="8">
+        <v>5</v>
+      </c>
+      <c r="K7" s="8">
+        <v>5</v>
+      </c>
       <c r="M7">
         <v>5</v>
       </c>
@@ -1028,10 +1044,21 @@
       <c r="E8" s="4">
         <v>5</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8" s="8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5</v>
+      </c>
+      <c r="K8" s="8">
+        <v>5</v>
+      </c>
       <c r="M8">
         <v>5</v>
       </c>
@@ -1039,6 +1066,9 @@
         <v>5</v>
       </c>
       <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
         <v>5</v>
       </c>
       <c r="Q8" s="4">
@@ -1610,9 +1640,18 @@
       <c r="F20" s="4">
         <v>5</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="H20" s="19">
+        <v>5</v>
+      </c>
+      <c r="I20" s="8">
+        <v>5</v>
+      </c>
+      <c r="J20" s="8">
+        <v>5</v>
+      </c>
+      <c r="K20" s="8">
+        <v>5</v>
+      </c>
       <c r="M20">
         <v>5</v>
       </c>
@@ -1936,9 +1975,24 @@
       <c r="F25" s="4">
         <v>5</v>
       </c>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="G25" s="6">
+        <v>5</v>
+      </c>
+      <c r="H25" s="19">
+        <v>5</v>
+      </c>
+      <c r="I25" s="8">
+        <v>5</v>
+      </c>
+      <c r="J25" s="8">
+        <v>5</v>
+      </c>
+      <c r="K25" s="8">
+        <v>5</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
       <c r="M25">
         <v>5</v>
       </c>
@@ -2003,9 +2057,24 @@
       <c r="F26" s="4">
         <v>5</v>
       </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="G26" s="6">
+        <v>5</v>
+      </c>
+      <c r="H26" s="19">
+        <v>5</v>
+      </c>
+      <c r="I26" s="8">
+        <v>5</v>
+      </c>
+      <c r="J26" s="8">
+        <v>5</v>
+      </c>
+      <c r="K26" s="8">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>5</v>
+      </c>
       <c r="M26">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 15:28:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -957,6 +957,9 @@
       <c r="Y6">
         <v>5</v>
       </c>
+      <c r="Z6">
+        <v>5</v>
+      </c>
       <c r="AD6">
         <v>24</v>
       </c>
@@ -1460,7 +1463,7 @@
       </c>
       <c r="S15" s="2"/>
       <c r="T15" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U15" s="8">
         <v>5</v>
@@ -2006,6 +2009,9 @@
         <v>5</v>
       </c>
       <c r="Q25" s="4">
+        <v>5</v>
+      </c>
+      <c r="R25">
         <v>5</v>
       </c>
       <c r="S25" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 15:36:35_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -638,7 +638,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1050,6 +1050,9 @@
       <c r="F8" s="2">
         <v>5</v>
       </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
       <c r="H8">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 15:45:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 16:01:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -635,10 +635,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q24" sqref="Q24"/>
+      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1211,9 +1211,33 @@
       <c r="Q10" s="4">
         <v>5</v>
       </c>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="8"/>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" s="2">
+        <v>5</v>
+      </c>
+      <c r="T10" s="2">
+        <v>5</v>
+      </c>
+      <c r="U10" s="8">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>5</v>
+      </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>5</v>
+      </c>
+      <c r="Y10">
+        <v>5</v>
+      </c>
+      <c r="Z10">
+        <v>5</v>
+      </c>
       <c r="AD10">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_10 июля 2024 г. 16:20:47_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
+++ b/2ОИБАС1222/2ОИБАС1222_ОпСис_.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
   <si>
     <t>Алигишиев Ибрагим</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>Л 11</t>
+  </si>
+  <si>
+    <t>И 13</t>
   </si>
 </sst>
 </file>
@@ -635,10 +638,10 @@
   <dimension ref="A1:AE55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q10" sqref="Q10"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -648,8 +651,9 @@
     <col min="3" max="3" width="29.1796875" customWidth="1"/>
     <col min="4" max="12" width="2.36328125" customWidth="1"/>
     <col min="13" max="15" width="3.26953125" customWidth="1"/>
-    <col min="16" max="16" width="4.81640625" customWidth="1"/>
-    <col min="17" max="18" width="2.453125" customWidth="1"/>
+    <col min="16" max="16" width="2.7265625" customWidth="1"/>
+    <col min="17" max="17" width="4.81640625" customWidth="1"/>
+    <col min="18" max="18" width="2.453125" customWidth="1"/>
     <col min="19" max="19" width="3.26953125" customWidth="1"/>
     <col min="20" max="23" width="2" customWidth="1"/>
     <col min="24" max="24" width="2.08984375" customWidth="1"/>
@@ -693,37 +697,40 @@
       <c r="O1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="P1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AD1" t="s">
@@ -742,10 +749,10 @@
       <c r="H2" s="3"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="3"/>
       <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
     </row>
     <row r="3" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -778,26 +785,26 @@
       <c r="O3">
         <v>5</v>
       </c>
-      <c r="Q3" s="4">
-        <v>5</v>
-      </c>
-      <c r="R3">
-        <v>5</v>
-      </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="4">
-        <v>5</v>
-      </c>
-      <c r="V3">
-        <v>5</v>
-      </c>
-      <c r="X3">
+      <c r="R3" s="4">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>5</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="4">
+        <v>5</v>
+      </c>
+      <c r="W3">
         <v>5</v>
       </c>
       <c r="Y3">
         <v>5</v>
       </c>
       <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
         <v>5</v>
       </c>
       <c r="AD3">
@@ -840,29 +847,29 @@
       <c r="O4">
         <v>5</v>
       </c>
-      <c r="Q4" s="4">
-        <v>5</v>
-      </c>
-      <c r="R4">
-        <v>5</v>
-      </c>
-      <c r="S4" s="2"/>
-      <c r="T4" s="4">
-        <v>5</v>
-      </c>
-      <c r="U4">
+      <c r="R4" s="4">
+        <v>5</v>
+      </c>
+      <c r="S4">
+        <v>5</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="4">
         <v>5</v>
       </c>
       <c r="V4">
         <v>5</v>
       </c>
-      <c r="X4">
+      <c r="W4">
         <v>5</v>
       </c>
       <c r="Y4">
         <v>5</v>
       </c>
       <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
         <v>5</v>
       </c>
       <c r="AD4">
@@ -893,11 +900,11 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-      <c r="Q5" s="4">
-        <v>5</v>
-      </c>
-      <c r="S5" s="2"/>
-      <c r="T5" s="4">
+      <c r="R5" s="4">
+        <v>5</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="U5" s="4">
         <v>3</v>
       </c>
       <c r="AD5">
@@ -935,19 +942,16 @@
       <c r="O6">
         <v>5</v>
       </c>
-      <c r="P6">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>5</v>
-      </c>
-      <c r="S6" s="2"/>
-      <c r="T6" s="4">
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6" s="4">
+        <v>5</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="U6" s="4">
         <v>4</v>
       </c>
-      <c r="V6">
-        <v>5</v>
-      </c>
       <c r="W6">
         <v>5</v>
       </c>
@@ -958,6 +962,9 @@
         <v>5</v>
       </c>
       <c r="Z6">
+        <v>5</v>
+      </c>
+      <c r="AA6">
         <v>5</v>
       </c>
       <c r="AD6">
@@ -1011,16 +1018,16 @@
       <c r="O7">
         <v>5</v>
       </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="4">
-        <v>5</v>
-      </c>
-      <c r="S7" s="2"/>
+      <c r="Q7">
+        <v>5</v>
+      </c>
+      <c r="R7" s="4">
+        <v>5</v>
+      </c>
       <c r="T7" s="2"/>
-      <c r="U7" s="8"/>
-      <c r="Z7">
+      <c r="U7" s="2"/>
+      <c r="V7" s="8"/>
+      <c r="AA7">
         <v>5</v>
       </c>
       <c r="AD7">
@@ -1074,23 +1081,20 @@
       <c r="O8">
         <v>5</v>
       </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-      <c r="Q8" s="4">
-        <v>5</v>
-      </c>
-      <c r="R8" s="5">
-        <v>5</v>
-      </c>
-      <c r="S8" s="2"/>
-      <c r="T8" s="4">
-        <v>5</v>
-      </c>
-      <c r="U8" s="8">
-        <v>5</v>
-      </c>
-      <c r="V8">
+      <c r="Q8">
+        <v>5</v>
+      </c>
+      <c r="R8" s="4">
+        <v>5</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="U8" s="4">
+        <v>5</v>
+      </c>
+      <c r="V8" s="8">
         <v>5</v>
       </c>
       <c r="W8">
@@ -1103,6 +1107,9 @@
         <v>5</v>
       </c>
       <c r="Z8">
+        <v>5</v>
+      </c>
+      <c r="AA8">
         <v>5</v>
       </c>
       <c r="AD8">
@@ -1150,20 +1157,17 @@
       <c r="O9">
         <v>5</v>
       </c>
-      <c r="P9">
-        <v>5</v>
-      </c>
-      <c r="Q9" s="4">
-        <v>5</v>
-      </c>
-      <c r="S9" s="2"/>
-      <c r="T9" s="4">
-        <v>5</v>
-      </c>
-      <c r="U9" s="8">
-        <v>5</v>
-      </c>
-      <c r="V9">
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9" s="4">
+        <v>5</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="U9" s="4">
+        <v>5</v>
+      </c>
+      <c r="V9" s="8">
         <v>5</v>
       </c>
       <c r="W9">
@@ -1176,6 +1180,9 @@
         <v>5</v>
       </c>
       <c r="Z9">
+        <v>5</v>
+      </c>
+      <c r="AA9">
         <v>5</v>
       </c>
       <c r="AD9">
@@ -1205,25 +1212,49 @@
       <c r="F10" s="4">
         <v>5</v>
       </c>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="Q10" s="4">
-        <v>5</v>
-      </c>
-      <c r="R10">
-        <v>5</v>
-      </c>
-      <c r="S10" s="2">
+      <c r="G10" s="6">
+        <v>5</v>
+      </c>
+      <c r="H10" s="19">
+        <v>5</v>
+      </c>
+      <c r="I10" s="8">
+        <v>5</v>
+      </c>
+      <c r="J10" s="8">
+        <v>5</v>
+      </c>
+      <c r="K10" s="8">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>5</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10">
+        <v>5</v>
+      </c>
+      <c r="R10" s="4">
+        <v>5</v>
+      </c>
+      <c r="S10">
         <v>5</v>
       </c>
       <c r="T10" s="2">
         <v>5</v>
       </c>
-      <c r="U10" s="8">
-        <v>5</v>
-      </c>
-      <c r="V10">
+      <c r="U10" s="2">
+        <v>5</v>
+      </c>
+      <c r="V10" s="8">
         <v>5</v>
       </c>
       <c r="W10">
@@ -1236,6 +1267,9 @@
         <v>5</v>
       </c>
       <c r="Z10">
+        <v>5</v>
+      </c>
+      <c r="AA10">
         <v>5</v>
       </c>
       <c r="AD10">
@@ -1276,26 +1310,26 @@
       <c r="O11">
         <v>5</v>
       </c>
-      <c r="Q11" s="4">
-        <v>5</v>
-      </c>
-      <c r="R11">
-        <v>5</v>
-      </c>
-      <c r="S11" s="2"/>
-      <c r="T11" s="4">
-        <v>5</v>
-      </c>
-      <c r="U11" s="8">
-        <v>5</v>
-      </c>
-      <c r="V11">
-        <v>5</v>
-      </c>
-      <c r="X11">
-        <v>5</v>
-      </c>
-      <c r="Z11">
+      <c r="R11" s="4">
+        <v>5</v>
+      </c>
+      <c r="S11">
+        <v>5</v>
+      </c>
+      <c r="T11" s="2"/>
+      <c r="U11" s="4">
+        <v>5</v>
+      </c>
+      <c r="V11" s="8">
+        <v>5</v>
+      </c>
+      <c r="W11">
+        <v>5</v>
+      </c>
+      <c r="Y11">
+        <v>5</v>
+      </c>
+      <c r="AA11">
         <v>5</v>
       </c>
       <c r="AD11">
@@ -1328,12 +1362,12 @@
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="Q12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="4">
-        <v>5</v>
-      </c>
-      <c r="U12" s="8"/>
+      <c r="R12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="4">
+        <v>5</v>
+      </c>
+      <c r="V12" s="8"/>
       <c r="AD12">
         <v>24</v>
       </c>
@@ -1373,21 +1407,18 @@
       <c r="O13">
         <v>5</v>
       </c>
-      <c r="P13">
-        <v>5</v>
-      </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="5">
-        <v>5</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="T13" s="4">
-        <v>5</v>
-      </c>
-      <c r="U13" s="8">
-        <v>5</v>
-      </c>
-      <c r="V13">
+      <c r="Q13">
+        <v>5</v>
+      </c>
+      <c r="R13" s="2"/>
+      <c r="S13" s="5">
+        <v>5</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="U13" s="4">
+        <v>5</v>
+      </c>
+      <c r="V13" s="8">
         <v>5</v>
       </c>
       <c r="W13">
@@ -1400,6 +1431,9 @@
         <v>5</v>
       </c>
       <c r="Z13">
+        <v>5</v>
+      </c>
+      <c r="AA13">
         <v>5</v>
       </c>
       <c r="AD13">
@@ -1432,12 +1466,12 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="Q14" s="4">
-        <v>5</v>
-      </c>
-      <c r="S14" s="2"/>
+      <c r="R14" s="4">
+        <v>5</v>
+      </c>
       <c r="T14" s="2"/>
-      <c r="U14" s="8"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="8"/>
       <c r="AD14">
         <v>3</v>
       </c>
@@ -1482,29 +1516,29 @@
       <c r="O15">
         <v>5</v>
       </c>
-      <c r="Q15" s="4">
-        <v>5</v>
-      </c>
-      <c r="R15">
-        <v>5</v>
-      </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="4">
-        <v>5</v>
-      </c>
-      <c r="U15" s="8">
-        <v>5</v>
-      </c>
-      <c r="V15">
-        <v>5</v>
-      </c>
-      <c r="X15">
+      <c r="R15" s="4">
+        <v>5</v>
+      </c>
+      <c r="S15">
+        <v>5</v>
+      </c>
+      <c r="T15" s="2"/>
+      <c r="U15" s="4">
+        <v>5</v>
+      </c>
+      <c r="V15" s="8">
+        <v>5</v>
+      </c>
+      <c r="W15">
         <v>5</v>
       </c>
       <c r="Y15">
         <v>5</v>
       </c>
       <c r="Z15">
+        <v>5</v>
+      </c>
+      <c r="AA15">
         <v>5</v>
       </c>
       <c r="AD15">
@@ -1539,14 +1573,14 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="Q16" s="4">
-        <v>5</v>
-      </c>
-      <c r="R16" s="5">
-        <v>5</v>
-      </c>
-      <c r="S16" s="2"/>
-      <c r="T16" s="4">
+      <c r="R16" s="4">
+        <v>5</v>
+      </c>
+      <c r="S16" s="5">
+        <v>5</v>
+      </c>
+      <c r="T16" s="2"/>
+      <c r="U16" s="4">
         <v>5</v>
       </c>
       <c r="AD16">
@@ -1570,9 +1604,9 @@
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="S17" s="12"/>
+      <c r="R17" s="12"/>
       <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
     </row>
     <row r="18" spans="1:31" s="11" customFormat="1" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -1588,9 +1622,9 @@
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
-      <c r="Q18" s="12"/>
-      <c r="S18" s="12"/>
+      <c r="R18" s="12"/>
       <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
     </row>
     <row r="19" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -1624,23 +1658,23 @@
       <c r="K19" s="4">
         <v>5</v>
       </c>
-      <c r="P19">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>5</v>
-      </c>
-      <c r="R19" s="7">
-        <v>5</v>
-      </c>
-      <c r="S19" s="2"/>
-      <c r="T19" s="4">
-        <v>5</v>
-      </c>
-      <c r="U19" s="8">
-        <v>5</v>
-      </c>
-      <c r="V19" s="19">
+      <c r="Q19">
+        <v>5</v>
+      </c>
+      <c r="R19" s="4">
+        <v>5</v>
+      </c>
+      <c r="S19" s="7">
+        <v>5</v>
+      </c>
+      <c r="T19" s="2"/>
+      <c r="U19" s="4">
+        <v>5</v>
+      </c>
+      <c r="V19" s="8">
+        <v>5</v>
+      </c>
+      <c r="W19" s="19">
         <v>5</v>
       </c>
       <c r="AD19">
@@ -1691,20 +1725,17 @@
       <c r="O20">
         <v>5</v>
       </c>
-      <c r="Q20" s="4">
-        <v>5</v>
-      </c>
-      <c r="R20">
-        <v>5</v>
-      </c>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2">
-        <v>5</v>
-      </c>
-      <c r="U20" s="8">
-        <v>5</v>
-      </c>
-      <c r="V20">
+      <c r="R20" s="4">
+        <v>5</v>
+      </c>
+      <c r="S20">
+        <v>5</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2">
+        <v>5</v>
+      </c>
+      <c r="V20" s="8">
         <v>5</v>
       </c>
       <c r="W20">
@@ -1717,6 +1748,9 @@
         <v>5</v>
       </c>
       <c r="Z20">
+        <v>5</v>
+      </c>
+      <c r="AA20">
         <v>5</v>
       </c>
       <c r="AD20">
@@ -1757,20 +1791,20 @@
       <c r="O21">
         <v>5</v>
       </c>
-      <c r="Q21" s="4">
-        <v>5</v>
-      </c>
-      <c r="S21" s="2"/>
-      <c r="T21" s="4">
-        <v>5</v>
-      </c>
-      <c r="U21" s="8">
-        <v>5</v>
-      </c>
-      <c r="X21">
+      <c r="R21" s="4">
+        <v>5</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="4">
+        <v>5</v>
+      </c>
+      <c r="V21" s="8">
         <v>5</v>
       </c>
       <c r="Y21">
+        <v>5</v>
+      </c>
+      <c r="Z21">
         <v>5</v>
       </c>
       <c r="AD21">
@@ -1801,17 +1835,17 @@
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-      <c r="Q22" s="4">
-        <v>5</v>
-      </c>
-      <c r="R22" s="5">
-        <v>5</v>
-      </c>
-      <c r="S22" s="2"/>
-      <c r="T22" s="4">
-        <v>5</v>
-      </c>
-      <c r="U22" s="8"/>
+      <c r="R22" s="4">
+        <v>5</v>
+      </c>
+      <c r="S22" s="5">
+        <v>5</v>
+      </c>
+      <c r="T22" s="2"/>
+      <c r="U22" s="4">
+        <v>5</v>
+      </c>
+      <c r="V22" s="8"/>
       <c r="AD22">
         <v>12</v>
       </c>
@@ -1854,6 +1888,9 @@
       <c r="K23" s="8">
         <v>5</v>
       </c>
+      <c r="L23" s="16">
+        <v>5</v>
+      </c>
       <c r="M23" s="8">
         <v>5</v>
       </c>
@@ -1863,28 +1900,28 @@
       <c r="O23">
         <v>5</v>
       </c>
-      <c r="P23">
-        <v>5</v>
-      </c>
-      <c r="Q23" s="4">
-        <v>5</v>
-      </c>
-      <c r="R23" s="5">
-        <v>5</v>
-      </c>
-      <c r="S23" s="4">
+      <c r="P23" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q23">
+        <v>5</v>
+      </c>
+      <c r="R23" s="4">
+        <v>5</v>
+      </c>
+      <c r="S23" s="5">
         <v>5</v>
       </c>
       <c r="T23" s="4">
         <v>5</v>
       </c>
-      <c r="U23" s="15">
-        <v>5</v>
-      </c>
-      <c r="V23" s="17">
-        <v>5</v>
-      </c>
-      <c r="W23">
+      <c r="U23" s="4">
+        <v>5</v>
+      </c>
+      <c r="V23" s="15">
+        <v>5</v>
+      </c>
+      <c r="W23" s="17">
         <v>5</v>
       </c>
       <c r="X23">
@@ -1894,6 +1931,9 @@
         <v>5</v>
       </c>
       <c r="Z23">
+        <v>5</v>
+      </c>
+      <c r="AA23">
         <v>5</v>
       </c>
       <c r="AD23">
@@ -1914,7 +1954,9 @@
       <c r="C24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
       <c r="E24" s="4">
         <v>5</v>
       </c>
@@ -1936,6 +1978,9 @@
       <c r="K24" s="4">
         <v>5</v>
       </c>
+      <c r="L24" s="6">
+        <v>5</v>
+      </c>
       <c r="M24" s="14">
         <v>5</v>
       </c>
@@ -1948,7 +1993,7 @@
       <c r="P24">
         <v>5</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24">
         <v>5</v>
       </c>
       <c r="R24" s="4">
@@ -1960,22 +2005,25 @@
       <c r="T24" s="4">
         <v>5</v>
       </c>
-      <c r="U24" s="16">
-        <v>5</v>
-      </c>
-      <c r="V24" s="14">
-        <v>5</v>
-      </c>
-      <c r="W24" s="19">
-        <v>5</v>
-      </c>
-      <c r="X24">
+      <c r="U24" s="4">
+        <v>5</v>
+      </c>
+      <c r="V24" s="16">
+        <v>5</v>
+      </c>
+      <c r="W24" s="14">
+        <v>5</v>
+      </c>
+      <c r="X24" s="19">
         <v>5</v>
       </c>
       <c r="Y24">
         <v>5</v>
       </c>
       <c r="Z24">
+        <v>5</v>
+      </c>
+      <c r="AA24">
         <v>5</v>
       </c>
       <c r="AD24">
@@ -2032,26 +2080,23 @@
       <c r="O25">
         <v>5</v>
       </c>
-      <c r="P25">
-        <v>5</v>
-      </c>
-      <c r="Q25" s="4">
-        <v>5</v>
-      </c>
-      <c r="R25">
-        <v>5</v>
-      </c>
-      <c r="S25" s="2"/>
-      <c r="T25" s="4">
-        <v>5</v>
-      </c>
-      <c r="U25" s="16">
-        <v>5</v>
-      </c>
-      <c r="V25" s="8">
-        <v>5</v>
-      </c>
-      <c r="W25">
+      <c r="Q25">
+        <v>5</v>
+      </c>
+      <c r="R25" s="4">
+        <v>5</v>
+      </c>
+      <c r="S25">
+        <v>5</v>
+      </c>
+      <c r="T25" s="2"/>
+      <c r="U25" s="4">
+        <v>5</v>
+      </c>
+      <c r="V25" s="16">
+        <v>5</v>
+      </c>
+      <c r="W25" s="8">
         <v>5</v>
       </c>
       <c r="X25">
@@ -2061,6 +2106,9 @@
         <v>5</v>
       </c>
       <c r="Z25">
+        <v>5</v>
+      </c>
+      <c r="AA25">
         <v>5</v>
       </c>
       <c r="AD25">
@@ -2117,26 +2165,23 @@
       <c r="O26">
         <v>5</v>
       </c>
-      <c r="P26">
-        <v>5</v>
-      </c>
-      <c r="Q26" s="4">
-        <v>5</v>
-      </c>
-      <c r="R26" s="5">
-        <v>5</v>
-      </c>
-      <c r="S26" s="2"/>
-      <c r="T26" s="4">
-        <v>5</v>
-      </c>
-      <c r="U26" s="16">
-        <v>5</v>
-      </c>
-      <c r="V26" s="8">
-        <v>5</v>
-      </c>
-      <c r="W26">
+      <c r="Q26">
+        <v>5</v>
+      </c>
+      <c r="R26" s="4">
+        <v>5</v>
+      </c>
+      <c r="S26" s="5">
+        <v>5</v>
+      </c>
+      <c r="T26" s="2"/>
+      <c r="U26" s="4">
+        <v>5</v>
+      </c>
+      <c r="V26" s="16">
+        <v>5</v>
+      </c>
+      <c r="W26" s="8">
         <v>5</v>
       </c>
       <c r="X26">
@@ -2146,6 +2191,9 @@
         <v>5</v>
       </c>
       <c r="Z26">
+        <v>5</v>
+      </c>
+      <c r="AA26">
         <v>5</v>
       </c>
       <c r="AD26">
@@ -2196,32 +2244,32 @@
       <c r="N27" s="13">
         <v>5</v>
       </c>
-      <c r="P27">
-        <v>5</v>
-      </c>
-      <c r="Q27" s="4">
-        <v>5</v>
-      </c>
-      <c r="R27" s="5">
-        <v>5</v>
-      </c>
-      <c r="S27" s="2"/>
-      <c r="T27" s="4">
-        <v>5</v>
-      </c>
-      <c r="U27" s="8">
+      <c r="Q27">
+        <v>5</v>
+      </c>
+      <c r="R27" s="4">
+        <v>5</v>
+      </c>
+      <c r="S27" s="5">
+        <v>5</v>
+      </c>
+      <c r="T27" s="2"/>
+      <c r="U27" s="4">
         <v>5</v>
       </c>
       <c r="V27" s="8">
         <v>5</v>
       </c>
-      <c r="X27">
+      <c r="W27" s="8">
         <v>5</v>
       </c>
       <c r="Y27">
         <v>5</v>
       </c>
       <c r="Z27">
+        <v>5</v>
+      </c>
+      <c r="AA27">
         <v>5</v>
       </c>
       <c r="AD27">
@@ -2255,23 +2303,23 @@
       <c r="N28" s="8">
         <v>5</v>
       </c>
-      <c r="P28">
-        <v>5</v>
-      </c>
-      <c r="Q28" s="4">
-        <v>5</v>
-      </c>
-      <c r="S28" s="2"/>
-      <c r="T28" s="4">
-        <v>5</v>
-      </c>
-      <c r="U28" s="16">
+      <c r="Q28">
+        <v>5</v>
+      </c>
+      <c r="R28" s="4">
+        <v>5</v>
+      </c>
+      <c r="T28" s="2"/>
+      <c r="U28" s="4">
         <v>5</v>
       </c>
       <c r="V28" s="16">
         <v>5</v>
       </c>
-      <c r="X28">
+      <c r="W28" s="16">
+        <v>5</v>
+      </c>
+      <c r="Y28">
         <v>5</v>
       </c>
       <c r="AD28">
@@ -2309,21 +2357,21 @@
       <c r="O29">
         <v>5</v>
       </c>
-      <c r="Q29" s="4">
-        <v>5</v>
-      </c>
-      <c r="S29" s="4">
-        <v>5</v>
-      </c>
-      <c r="T29" s="2"/>
-      <c r="U29" s="16"/>
-      <c r="V29" s="16">
-        <v>5</v>
-      </c>
-      <c r="W29">
+      <c r="R29" s="4">
+        <v>5</v>
+      </c>
+      <c r="T29" s="4">
+        <v>5</v>
+      </c>
+      <c r="U29" s="2"/>
+      <c r="V29" s="16"/>
+      <c r="W29" s="16">
         <v>5</v>
       </c>
       <c r="X29">
+        <v>5</v>
+      </c>
+      <c r="Y29">
         <v>5</v>
       </c>
       <c r="AD29">
@@ -2374,32 +2422,32 @@
       <c r="O30">
         <v>5</v>
       </c>
-      <c r="P30">
-        <v>5</v>
-      </c>
-      <c r="Q30" s="4">
-        <v>5</v>
-      </c>
-      <c r="R30" s="6">
-        <v>5</v>
-      </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="4">
-        <v>5</v>
-      </c>
-      <c r="U30" s="8">
-        <v>5</v>
-      </c>
-      <c r="V30" s="14">
-        <v>5</v>
-      </c>
-      <c r="X30">
+      <c r="Q30">
+        <v>5</v>
+      </c>
+      <c r="R30" s="4">
+        <v>5</v>
+      </c>
+      <c r="S30" s="6">
+        <v>5</v>
+      </c>
+      <c r="T30" s="2"/>
+      <c r="U30" s="4">
+        <v>5</v>
+      </c>
+      <c r="V30" s="8">
+        <v>5</v>
+      </c>
+      <c r="W30" s="14">
         <v>5</v>
       </c>
       <c r="Y30">
         <v>5</v>
       </c>
       <c r="Z30">
+        <v>5</v>
+      </c>
+      <c r="AA30">
         <v>5</v>
       </c>
       <c r="AD30">
@@ -2419,11 +2467,11 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="6"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="4"/>
-      <c r="U31" s="8"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="4"/>
+      <c r="V31" s="8"/>
     </row>
     <row r="32" spans="1:31" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
@@ -2435,12 +2483,12 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="4"/>
-    </row>
-    <row r="33" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="4"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="4"/>
+    </row>
+    <row r="33" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -2450,12 +2498,12 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="4"/>
-    </row>
-    <row r="34" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="4"/>
+      <c r="S33" s="6"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="4"/>
+    </row>
+    <row r="34" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="1"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -2470,7 +2518,7 @@
       <c r="S34" s="2"/>
       <c r="T34" s="4"/>
     </row>
-    <row r="35" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="1"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -2485,7 +2533,7 @@
       <c r="S35" s="2"/>
       <c r="T35" s="4"/>
     </row>
-    <row r="36" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="1"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2500,7 +2548,7 @@
       <c r="S36" s="2"/>
       <c r="T36" s="4"/>
     </row>
-    <row r="37" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="1"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -2515,7 +2563,7 @@
       <c r="S37" s="2"/>
       <c r="T37" s="4"/>
     </row>
-    <row r="38" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="1"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -2530,7 +2578,7 @@
       <c r="S38" s="2"/>
       <c r="T38" s="4"/>
     </row>
-    <row r="39" spans="3:20" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:21" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="1"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -2545,33 +2593,33 @@
       <c r="S39" s="2"/>
       <c r="T39" s="4"/>
     </row>
-    <row r="40" spans="3:20" ht="13" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:21" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
     </row>
-    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:21" x14ac:dyDescent="0.25">
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:21" x14ac:dyDescent="0.25">
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:21" x14ac:dyDescent="0.25">
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:21" x14ac:dyDescent="0.25">
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H45" s="8"/>
     </row>
-    <row r="46" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H46" s="8"/>
     </row>
-    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H47" s="8"/>
     </row>
-    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:21" x14ac:dyDescent="0.25">
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.25">

</xml_diff>